<commit_message>
Enhanced time tracking file
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -27,6 +27,12 @@
   </si>
   <si>
     <t>Created basic project with basic movements (with unity pathfinding)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Sub-total</t>
   </si>
 </sst>
 </file>
@@ -477,20 +483,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D200"/>
+  <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="100.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -500,8 +506,14 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
         <v>42300</v>
       </c>
@@ -511,991 +523,1787 @@
       <c r="D3" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <f>IF(D3="", "", SUM(D$3:D3))</f>
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="1">
+        <f>SUM(D3:D200)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="str">
+        <f>IF(D4="", "", SUM(D$3:D4))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="str">
+        <f>IF(D5="", "", SUM(D$3:D5))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="str">
+        <f>IF(D6="", "", SUM(D$3:D6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="str">
+        <f>IF(D7="", "", SUM(D$3:D7))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="str">
+        <f>IF(D8="", "", SUM(D$3:D8))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="str">
+        <f>IF(D9="", "", SUM(D$3:D9))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="str">
+        <f>IF(D10="", "", SUM(D$3:D10))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="str">
+        <f>IF(D11="", "", SUM(D$3:D11))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="str">
+        <f>IF(D12="", "", SUM(D$3:D12))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="str">
+        <f>IF(D13="", "", SUM(D$3:D13))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="str">
+        <f>IF(D14="", "", SUM(D$3:D14))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="str">
+        <f>IF(D15="", "", SUM(D$3:D15))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="str">
+        <f>IF(D16="", "", SUM(D$3:D16))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="str">
+        <f>IF(D17="", "", SUM(D$3:D17))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="4"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="str">
+        <f>IF(D18="", "", SUM(D$3:D18))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="str">
+        <f>IF(D19="", "", SUM(D$3:D19))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="str">
+        <f>IF(D20="", "", SUM(D$3:D20))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="4"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="str">
+        <f>IF(D21="", "", SUM(D$3:D21))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="str">
+        <f>IF(D22="", "", SUM(D$3:D22))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="str">
+        <f>IF(D23="", "", SUM(D$3:D23))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="4"/>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="str">
+        <f>IF(D24="", "", SUM(D$3:D24))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="C25" s="4"/>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="str">
+        <f>IF(D25="", "", SUM(D$3:D25))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="4"/>
       <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="str">
+        <f>IF(D26="", "", SUM(D$3:D26))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="C27" s="4"/>
       <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="str">
+        <f>IF(D27="", "", SUM(D$3:D27))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="C28" s="4"/>
       <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="str">
+        <f>IF(D28="", "", SUM(D$3:D28))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="4"/>
       <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="str">
+        <f>IF(D29="", "", SUM(D$3:D29))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="4"/>
       <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="str">
+        <f>IF(D30="", "", SUM(D$3:D30))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="4"/>
       <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="str">
+        <f>IF(D31="", "", SUM(D$3:D31))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="4"/>
       <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="str">
+        <f>IF(D32="", "", SUM(D$3:D32))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="C33" s="4"/>
       <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="str">
+        <f>IF(D33="", "", SUM(D$3:D33))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="4"/>
       <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="str">
+        <f>IF(D34="", "", SUM(D$3:D34))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="4"/>
       <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="str">
+        <f>IF(D35="", "", SUM(D$3:D35))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="4"/>
       <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="str">
+        <f>IF(D36="", "", SUM(D$3:D36))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="C37" s="4"/>
       <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="str">
+        <f>IF(D37="", "", SUM(D$3:D37))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="4"/>
       <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="1" t="str">
+        <f>IF(D38="", "", SUM(D$3:D38))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="C39" s="4"/>
       <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="1" t="str">
+        <f>IF(D39="", "", SUM(D$3:D39))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="C40" s="4"/>
       <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="str">
+        <f>IF(D40="", "", SUM(D$3:D40))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="C41" s="4"/>
       <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="str">
+        <f>IF(D41="", "", SUM(D$3:D41))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="4"/>
       <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E42" s="1" t="str">
+        <f>IF(D42="", "", SUM(D$3:D42))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="4"/>
       <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="str">
+        <f>IF(D43="", "", SUM(D$3:D43))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="C44" s="4"/>
       <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E44" s="1" t="str">
+        <f>IF(D44="", "", SUM(D$3:D44))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="C45" s="4"/>
       <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="1" t="str">
+        <f>IF(D45="", "", SUM(D$3:D45))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="C46" s="4"/>
       <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="str">
+        <f>IF(D46="", "", SUM(D$3:D46))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="C47" s="4"/>
       <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="str">
+        <f>IF(D47="", "", SUM(D$3:D47))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="C48" s="4"/>
       <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="str">
+        <f>IF(D48="", "", SUM(D$3:D48))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="C49" s="4"/>
       <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E49" s="1" t="str">
+        <f>IF(D49="", "", SUM(D$3:D49))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="4"/>
       <c r="D50" s="1"/>
-    </row>
-    <row r="51" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="1" t="str">
+        <f>IF(D50="", "", SUM(D$3:D50))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="C51" s="4"/>
       <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E51" s="1" t="str">
+        <f>IF(D51="", "", SUM(D$3:D51))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="C52" s="4"/>
       <c r="D52" s="1"/>
-    </row>
-    <row r="53" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="1" t="str">
+        <f>IF(D52="", "", SUM(D$3:D52))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="C53" s="4"/>
       <c r="D53" s="1"/>
-    </row>
-    <row r="54" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E53" s="1" t="str">
+        <f>IF(D53="", "", SUM(D$3:D53))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="C54" s="4"/>
       <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="str">
+        <f>IF(D54="", "", SUM(D$3:D54))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="4"/>
       <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="1" t="str">
+        <f>IF(D55="", "", SUM(D$3:D55))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="C56" s="4"/>
       <c r="D56" s="1"/>
-    </row>
-    <row r="57" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E56" s="1" t="str">
+        <f>IF(D56="", "", SUM(D$3:D56))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="C57" s="4"/>
       <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="1" t="str">
+        <f>IF(D57="", "", SUM(D$3:D57))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="C58" s="4"/>
       <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="str">
+        <f>IF(D58="", "", SUM(D$3:D58))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="C59" s="4"/>
       <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="str">
+        <f>IF(D59="", "", SUM(D$3:D59))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="C60" s="4"/>
       <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E60" s="1" t="str">
+        <f>IF(D60="", "", SUM(D$3:D60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="C61" s="4"/>
       <c r="D61" s="1"/>
-    </row>
-    <row r="62" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E61" s="1" t="str">
+        <f>IF(D61="", "", SUM(D$3:D61))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="C62" s="4"/>
       <c r="D62" s="1"/>
-    </row>
-    <row r="63" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="str">
+        <f>IF(D62="", "", SUM(D$3:D62))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="C63" s="4"/>
       <c r="D63" s="1"/>
-    </row>
-    <row r="64" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E63" s="1" t="str">
+        <f>IF(D63="", "", SUM(D$3:D63))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
       <c r="C64" s="4"/>
       <c r="D64" s="1"/>
-    </row>
-    <row r="65" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E64" s="1" t="str">
+        <f>IF(D64="", "", SUM(D$3:D64))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="C65" s="4"/>
       <c r="D65" s="1"/>
-    </row>
-    <row r="66" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E65" s="1" t="str">
+        <f>IF(D65="", "", SUM(D$3:D65))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="C66" s="4"/>
       <c r="D66" s="1"/>
-    </row>
-    <row r="67" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E66" s="1" t="str">
+        <f>IF(D66="", "", SUM(D$3:D66))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="C67" s="4"/>
       <c r="D67" s="1"/>
-    </row>
-    <row r="68" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E67" s="1" t="str">
+        <f>IF(D67="", "", SUM(D$3:D67))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="C68" s="4"/>
       <c r="D68" s="1"/>
-    </row>
-    <row r="69" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E68" s="1" t="str">
+        <f>IF(D68="", "", SUM(D$3:D68))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="C69" s="4"/>
       <c r="D69" s="1"/>
-    </row>
-    <row r="70" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E69" s="1" t="str">
+        <f>IF(D69="", "", SUM(D$3:D69))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="C70" s="4"/>
       <c r="D70" s="1"/>
-    </row>
-    <row r="71" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E70" s="1" t="str">
+        <f>IF(D70="", "", SUM(D$3:D70))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="C71" s="4"/>
       <c r="D71" s="1"/>
-    </row>
-    <row r="72" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E71" s="1" t="str">
+        <f>IF(D71="", "", SUM(D$3:D71))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="C72" s="4"/>
       <c r="D72" s="1"/>
-    </row>
-    <row r="73" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E72" s="1" t="str">
+        <f>IF(D72="", "", SUM(D$3:D72))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="C73" s="4"/>
       <c r="D73" s="1"/>
-    </row>
-    <row r="74" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="1" t="str">
+        <f>IF(D73="", "", SUM(D$3:D73))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
       <c r="C74" s="4"/>
       <c r="D74" s="1"/>
-    </row>
-    <row r="75" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E74" s="1" t="str">
+        <f>IF(D74="", "", SUM(D$3:D74))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="C75" s="4"/>
       <c r="D75" s="1"/>
-    </row>
-    <row r="76" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E75" s="1" t="str">
+        <f>IF(D75="", "", SUM(D$3:D75))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
       <c r="C76" s="4"/>
       <c r="D76" s="1"/>
-    </row>
-    <row r="77" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E76" s="1" t="str">
+        <f>IF(D76="", "", SUM(D$3:D76))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="C77" s="4"/>
       <c r="D77" s="1"/>
-    </row>
-    <row r="78" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E77" s="1" t="str">
+        <f>IF(D77="", "", SUM(D$3:D77))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="C78" s="4"/>
       <c r="D78" s="1"/>
-    </row>
-    <row r="79" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E78" s="1" t="str">
+        <f>IF(D78="", "", SUM(D$3:D78))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="C79" s="4"/>
       <c r="D79" s="1"/>
-    </row>
-    <row r="80" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E79" s="1" t="str">
+        <f>IF(D79="", "", SUM(D$3:D79))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="C80" s="4"/>
       <c r="D80" s="1"/>
-    </row>
-    <row r="81" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E80" s="1" t="str">
+        <f>IF(D80="", "", SUM(D$3:D80))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="C81" s="4"/>
       <c r="D81" s="1"/>
-    </row>
-    <row r="82" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E81" s="1" t="str">
+        <f>IF(D81="", "", SUM(D$3:D81))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="C82" s="4"/>
       <c r="D82" s="1"/>
-    </row>
-    <row r="83" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E82" s="1" t="str">
+        <f>IF(D82="", "", SUM(D$3:D82))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="C83" s="4"/>
       <c r="D83" s="1"/>
-    </row>
-    <row r="84" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E83" s="1" t="str">
+        <f>IF(D83="", "", SUM(D$3:D83))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="C84" s="4"/>
       <c r="D84" s="1"/>
-    </row>
-    <row r="85" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E84" s="1" t="str">
+        <f>IF(D84="", "", SUM(D$3:D84))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="C85" s="4"/>
       <c r="D85" s="1"/>
-    </row>
-    <row r="86" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E85" s="1" t="str">
+        <f>IF(D85="", "", SUM(D$3:D85))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="C86" s="4"/>
       <c r="D86" s="1"/>
-    </row>
-    <row r="87" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E86" s="1" t="str">
+        <f>IF(D86="", "", SUM(D$3:D86))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="C87" s="4"/>
       <c r="D87" s="1"/>
-    </row>
-    <row r="88" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E87" s="1" t="str">
+        <f>IF(D87="", "", SUM(D$3:D87))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
       <c r="C88" s="4"/>
       <c r="D88" s="1"/>
-    </row>
-    <row r="89" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E88" s="1" t="str">
+        <f>IF(D88="", "", SUM(D$3:D88))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="C89" s="4"/>
       <c r="D89" s="1"/>
-    </row>
-    <row r="90" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E89" s="1" t="str">
+        <f>IF(D89="", "", SUM(D$3:D89))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
       <c r="C90" s="4"/>
       <c r="D90" s="1"/>
-    </row>
-    <row r="91" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E90" s="1" t="str">
+        <f>IF(D90="", "", SUM(D$3:D90))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="6"/>
       <c r="C91" s="4"/>
       <c r="D91" s="1"/>
-    </row>
-    <row r="92" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E91" s="1" t="str">
+        <f>IF(D91="", "", SUM(D$3:D91))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
       <c r="C92" s="4"/>
       <c r="D92" s="1"/>
-    </row>
-    <row r="93" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E92" s="1" t="str">
+        <f>IF(D92="", "", SUM(D$3:D92))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
       <c r="C93" s="4"/>
       <c r="D93" s="1"/>
-    </row>
-    <row r="94" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E93" s="1" t="str">
+        <f>IF(D93="", "", SUM(D$3:D93))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="6"/>
       <c r="C94" s="4"/>
       <c r="D94" s="1"/>
-    </row>
-    <row r="95" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E94" s="1" t="str">
+        <f>IF(D94="", "", SUM(D$3:D94))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
       <c r="C95" s="4"/>
       <c r="D95" s="1"/>
-    </row>
-    <row r="96" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E95" s="1" t="str">
+        <f>IF(D95="", "", SUM(D$3:D95))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="6"/>
       <c r="C96" s="4"/>
       <c r="D96" s="1"/>
-    </row>
-    <row r="97" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E96" s="1" t="str">
+        <f>IF(D96="", "", SUM(D$3:D96))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
       <c r="C97" s="4"/>
       <c r="D97" s="1"/>
-    </row>
-    <row r="98" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E97" s="1" t="str">
+        <f>IF(D97="", "", SUM(D$3:D97))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
       <c r="C98" s="4"/>
       <c r="D98" s="1"/>
-    </row>
-    <row r="99" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E98" s="1" t="str">
+        <f>IF(D98="", "", SUM(D$3:D98))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
       <c r="C99" s="4"/>
       <c r="D99" s="1"/>
-    </row>
-    <row r="100" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E99" s="1" t="str">
+        <f>IF(D99="", "", SUM(D$3:D99))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
       <c r="C100" s="4"/>
       <c r="D100" s="1"/>
-    </row>
-    <row r="101" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E100" s="1" t="str">
+        <f>IF(D100="", "", SUM(D$3:D100))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
       <c r="C101" s="4"/>
       <c r="D101" s="1"/>
-    </row>
-    <row r="102" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E101" s="1" t="str">
+        <f>IF(D101="", "", SUM(D$3:D101))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="6"/>
       <c r="C102" s="4"/>
       <c r="D102" s="1"/>
-    </row>
-    <row r="103" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E102" s="1" t="str">
+        <f>IF(D102="", "", SUM(D$3:D102))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="6"/>
       <c r="C103" s="4"/>
       <c r="D103" s="1"/>
-    </row>
-    <row r="104" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E103" s="1" t="str">
+        <f>IF(D103="", "", SUM(D$3:D103))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
       <c r="C104" s="4"/>
       <c r="D104" s="1"/>
-    </row>
-    <row r="105" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E104" s="1" t="str">
+        <f>IF(D104="", "", SUM(D$3:D104))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="6"/>
       <c r="C105" s="4"/>
       <c r="D105" s="1"/>
-    </row>
-    <row r="106" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E105" s="1" t="str">
+        <f>IF(D105="", "", SUM(D$3:D105))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="6"/>
       <c r="C106" s="4"/>
       <c r="D106" s="1"/>
-    </row>
-    <row r="107" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E106" s="1" t="str">
+        <f>IF(D106="", "", SUM(D$3:D106))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="6"/>
       <c r="C107" s="4"/>
       <c r="D107" s="1"/>
-    </row>
-    <row r="108" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E107" s="1" t="str">
+        <f>IF(D107="", "", SUM(D$3:D107))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="6"/>
       <c r="C108" s="4"/>
       <c r="D108" s="1"/>
-    </row>
-    <row r="109" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E108" s="1" t="str">
+        <f>IF(D108="", "", SUM(D$3:D108))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="6"/>
       <c r="C109" s="4"/>
       <c r="D109" s="1"/>
-    </row>
-    <row r="110" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E109" s="1" t="str">
+        <f>IF(D109="", "", SUM(D$3:D109))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="6"/>
       <c r="C110" s="4"/>
       <c r="D110" s="1"/>
-    </row>
-    <row r="111" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E110" s="1" t="str">
+        <f>IF(D110="", "", SUM(D$3:D110))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="6"/>
       <c r="C111" s="4"/>
       <c r="D111" s="1"/>
-    </row>
-    <row r="112" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E111" s="1" t="str">
+        <f>IF(D111="", "", SUM(D$3:D111))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="6"/>
       <c r="C112" s="4"/>
       <c r="D112" s="1"/>
-    </row>
-    <row r="113" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E112" s="1" t="str">
+        <f>IF(D112="", "", SUM(D$3:D112))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="6"/>
       <c r="C113" s="4"/>
       <c r="D113" s="1"/>
-    </row>
-    <row r="114" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E113" s="1" t="str">
+        <f>IF(D113="", "", SUM(D$3:D113))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="6"/>
       <c r="C114" s="4"/>
       <c r="D114" s="1"/>
-    </row>
-    <row r="115" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E114" s="1" t="str">
+        <f>IF(D114="", "", SUM(D$3:D114))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="6"/>
       <c r="C115" s="4"/>
       <c r="D115" s="1"/>
-    </row>
-    <row r="116" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E115" s="1" t="str">
+        <f>IF(D115="", "", SUM(D$3:D115))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="6"/>
       <c r="C116" s="4"/>
       <c r="D116" s="1"/>
-    </row>
-    <row r="117" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E116" s="1" t="str">
+        <f>IF(D116="", "", SUM(D$3:D116))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="6"/>
       <c r="C117" s="4"/>
       <c r="D117" s="1"/>
-    </row>
-    <row r="118" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E117" s="1" t="str">
+        <f>IF(D117="", "", SUM(D$3:D117))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="6"/>
       <c r="C118" s="4"/>
       <c r="D118" s="1"/>
-    </row>
-    <row r="119" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E118" s="1" t="str">
+        <f>IF(D118="", "", SUM(D$3:D118))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="6"/>
       <c r="C119" s="4"/>
       <c r="D119" s="1"/>
-    </row>
-    <row r="120" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E119" s="1" t="str">
+        <f>IF(D119="", "", SUM(D$3:D119))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="6"/>
       <c r="C120" s="4"/>
       <c r="D120" s="1"/>
-    </row>
-    <row r="121" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E120" s="1" t="str">
+        <f>IF(D120="", "", SUM(D$3:D120))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="6"/>
       <c r="C121" s="4"/>
       <c r="D121" s="1"/>
-    </row>
-    <row r="122" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E121" s="1" t="str">
+        <f>IF(D121="", "", SUM(D$3:D121))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="6"/>
       <c r="C122" s="4"/>
       <c r="D122" s="1"/>
-    </row>
-    <row r="123" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E122" s="1" t="str">
+        <f>IF(D122="", "", SUM(D$3:D122))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="6"/>
       <c r="C123" s="4"/>
       <c r="D123" s="1"/>
-    </row>
-    <row r="124" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E123" s="1" t="str">
+        <f>IF(D123="", "", SUM(D$3:D123))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="6"/>
       <c r="C124" s="4"/>
       <c r="D124" s="1"/>
-    </row>
-    <row r="125" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E124" s="1" t="str">
+        <f>IF(D124="", "", SUM(D$3:D124))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
       <c r="C125" s="4"/>
       <c r="D125" s="1"/>
-    </row>
-    <row r="126" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E125" s="1" t="str">
+        <f>IF(D125="", "", SUM(D$3:D125))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="6"/>
       <c r="C126" s="4"/>
       <c r="D126" s="1"/>
-    </row>
-    <row r="127" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E126" s="1" t="str">
+        <f>IF(D126="", "", SUM(D$3:D126))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="6"/>
       <c r="C127" s="4"/>
       <c r="D127" s="1"/>
-    </row>
-    <row r="128" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E127" s="1" t="str">
+        <f>IF(D127="", "", SUM(D$3:D127))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="6"/>
       <c r="C128" s="4"/>
       <c r="D128" s="1"/>
-    </row>
-    <row r="129" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E128" s="1" t="str">
+        <f>IF(D128="", "", SUM(D$3:D128))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="6"/>
       <c r="C129" s="4"/>
       <c r="D129" s="1"/>
-    </row>
-    <row r="130" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E129" s="1" t="str">
+        <f>IF(D129="", "", SUM(D$3:D129))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="6"/>
       <c r="C130" s="4"/>
       <c r="D130" s="1"/>
-    </row>
-    <row r="131" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E130" s="1" t="str">
+        <f>IF(D130="", "", SUM(D$3:D130))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="6"/>
       <c r="C131" s="4"/>
       <c r="D131" s="1"/>
-    </row>
-    <row r="132" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E131" s="1" t="str">
+        <f>IF(D131="", "", SUM(D$3:D131))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
       <c r="C132" s="4"/>
       <c r="D132" s="1"/>
-    </row>
-    <row r="133" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E132" s="1" t="str">
+        <f>IF(D132="", "", SUM(D$3:D132))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
       <c r="C133" s="4"/>
       <c r="D133" s="1"/>
-    </row>
-    <row r="134" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E133" s="1" t="str">
+        <f>IF(D133="", "", SUM(D$3:D133))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="6"/>
       <c r="C134" s="4"/>
       <c r="D134" s="1"/>
-    </row>
-    <row r="135" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E134" s="1" t="str">
+        <f>IF(D134="", "", SUM(D$3:D134))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
       <c r="C135" s="4"/>
       <c r="D135" s="1"/>
-    </row>
-    <row r="136" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E135" s="1" t="str">
+        <f>IF(D135="", "", SUM(D$3:D135))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
       <c r="C136" s="4"/>
       <c r="D136" s="1"/>
-    </row>
-    <row r="137" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E136" s="1" t="str">
+        <f>IF(D136="", "", SUM(D$3:D136))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="6"/>
       <c r="C137" s="4"/>
       <c r="D137" s="1"/>
-    </row>
-    <row r="138" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E137" s="1" t="str">
+        <f>IF(D137="", "", SUM(D$3:D137))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
       <c r="C138" s="4"/>
       <c r="D138" s="1"/>
-    </row>
-    <row r="139" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E138" s="1" t="str">
+        <f>IF(D138="", "", SUM(D$3:D138))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="6"/>
       <c r="C139" s="4"/>
       <c r="D139" s="1"/>
-    </row>
-    <row r="140" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E139" s="1" t="str">
+        <f>IF(D139="", "", SUM(D$3:D139))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
       <c r="C140" s="4"/>
       <c r="D140" s="1"/>
-    </row>
-    <row r="141" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E140" s="1" t="str">
+        <f>IF(D140="", "", SUM(D$3:D140))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
       <c r="C141" s="4"/>
       <c r="D141" s="1"/>
-    </row>
-    <row r="142" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E141" s="1" t="str">
+        <f>IF(D141="", "", SUM(D$3:D141))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
       <c r="C142" s="4"/>
       <c r="D142" s="1"/>
-    </row>
-    <row r="143" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E142" s="1" t="str">
+        <f>IF(D142="", "", SUM(D$3:D142))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="6"/>
       <c r="C143" s="4"/>
       <c r="D143" s="1"/>
-    </row>
-    <row r="144" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E143" s="1" t="str">
+        <f>IF(D143="", "", SUM(D$3:D143))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
       <c r="C144" s="4"/>
       <c r="D144" s="1"/>
-    </row>
-    <row r="145" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E144" s="1" t="str">
+        <f>IF(D144="", "", SUM(D$3:D144))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
       <c r="C145" s="4"/>
       <c r="D145" s="1"/>
-    </row>
-    <row r="146" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E145" s="1" t="str">
+        <f>IF(D145="", "", SUM(D$3:D145))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
       <c r="C146" s="4"/>
       <c r="D146" s="1"/>
-    </row>
-    <row r="147" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E146" s="1" t="str">
+        <f>IF(D146="", "", SUM(D$3:D146))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="6"/>
       <c r="C147" s="4"/>
       <c r="D147" s="1"/>
-    </row>
-    <row r="148" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E147" s="1" t="str">
+        <f>IF(D147="", "", SUM(D$3:D147))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="6"/>
       <c r="C148" s="4"/>
       <c r="D148" s="1"/>
-    </row>
-    <row r="149" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E148" s="1" t="str">
+        <f>IF(D148="", "", SUM(D$3:D148))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
       <c r="C149" s="4"/>
       <c r="D149" s="1"/>
-    </row>
-    <row r="150" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E149" s="1" t="str">
+        <f>IF(D149="", "", SUM(D$3:D149))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="6"/>
       <c r="C150" s="4"/>
       <c r="D150" s="1"/>
-    </row>
-    <row r="151" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E150" s="1" t="str">
+        <f>IF(D150="", "", SUM(D$3:D150))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="6"/>
       <c r="C151" s="4"/>
       <c r="D151" s="1"/>
-    </row>
-    <row r="152" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E151" s="1" t="str">
+        <f>IF(D151="", "", SUM(D$3:D151))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="6"/>
       <c r="C152" s="4"/>
       <c r="D152" s="1"/>
-    </row>
-    <row r="153" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E152" s="1" t="str">
+        <f>IF(D152="", "", SUM(D$3:D152))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
       <c r="C153" s="4"/>
       <c r="D153" s="1"/>
-    </row>
-    <row r="154" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E153" s="1" t="str">
+        <f>IF(D153="", "", SUM(D$3:D153))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="6"/>
       <c r="C154" s="4"/>
       <c r="D154" s="1"/>
-    </row>
-    <row r="155" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E154" s="1" t="str">
+        <f>IF(D154="", "", SUM(D$3:D154))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="6"/>
       <c r="C155" s="4"/>
       <c r="D155" s="1"/>
-    </row>
-    <row r="156" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E155" s="1" t="str">
+        <f>IF(D155="", "", SUM(D$3:D155))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="6"/>
       <c r="C156" s="4"/>
       <c r="D156" s="1"/>
-    </row>
-    <row r="157" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E156" s="1" t="str">
+        <f>IF(D156="", "", SUM(D$3:D156))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
       <c r="C157" s="4"/>
       <c r="D157" s="1"/>
-    </row>
-    <row r="158" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E157" s="1" t="str">
+        <f>IF(D157="", "", SUM(D$3:D157))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
       <c r="C158" s="4"/>
       <c r="D158" s="1"/>
-    </row>
-    <row r="159" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E158" s="1" t="str">
+        <f>IF(D158="", "", SUM(D$3:D158))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="6"/>
       <c r="C159" s="4"/>
       <c r="D159" s="1"/>
-    </row>
-    <row r="160" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E159" s="1" t="str">
+        <f>IF(D159="", "", SUM(D$3:D159))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
       <c r="C160" s="4"/>
       <c r="D160" s="1"/>
-    </row>
-    <row r="161" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E160" s="1" t="str">
+        <f>IF(D160="", "", SUM(D$3:D160))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="161" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
       <c r="C161" s="4"/>
       <c r="D161" s="1"/>
-    </row>
-    <row r="162" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E161" s="1" t="str">
+        <f>IF(D161="", "", SUM(D$3:D161))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="162" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
       <c r="C162" s="4"/>
       <c r="D162" s="1"/>
-    </row>
-    <row r="163" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E162" s="1" t="str">
+        <f>IF(D162="", "", SUM(D$3:D162))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="163" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>
       <c r="C163" s="4"/>
       <c r="D163" s="1"/>
-    </row>
-    <row r="164" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E163" s="1" t="str">
+        <f>IF(D163="", "", SUM(D$3:D163))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="164" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
       <c r="C164" s="4"/>
       <c r="D164" s="1"/>
-    </row>
-    <row r="165" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E164" s="1" t="str">
+        <f>IF(D164="", "", SUM(D$3:D164))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="165" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
       <c r="C165" s="4"/>
       <c r="D165" s="1"/>
-    </row>
-    <row r="166" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E165" s="1" t="str">
+        <f>IF(D165="", "", SUM(D$3:D165))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="166" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
       <c r="C166" s="4"/>
       <c r="D166" s="1"/>
-    </row>
-    <row r="167" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E166" s="1" t="str">
+        <f>IF(D166="", "", SUM(D$3:D166))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="167" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="6"/>
       <c r="C167" s="4"/>
       <c r="D167" s="1"/>
-    </row>
-    <row r="168" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E167" s="1" t="str">
+        <f>IF(D167="", "", SUM(D$3:D167))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="6"/>
       <c r="C168" s="4"/>
       <c r="D168" s="1"/>
-    </row>
-    <row r="169" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E168" s="1" t="str">
+        <f>IF(D168="", "", SUM(D$3:D168))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="169" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
       <c r="C169" s="4"/>
       <c r="D169" s="1"/>
-    </row>
-    <row r="170" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E169" s="1" t="str">
+        <f>IF(D169="", "", SUM(D$3:D169))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
       <c r="C170" s="4"/>
       <c r="D170" s="1"/>
-    </row>
-    <row r="171" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E170" s="1" t="str">
+        <f>IF(D170="", "", SUM(D$3:D170))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
       <c r="C171" s="4"/>
       <c r="D171" s="1"/>
-    </row>
-    <row r="172" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E171" s="1" t="str">
+        <f>IF(D171="", "", SUM(D$3:D171))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="172" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="6"/>
       <c r="C172" s="4"/>
       <c r="D172" s="1"/>
-    </row>
-    <row r="173" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E172" s="1" t="str">
+        <f>IF(D172="", "", SUM(D$3:D172))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="173" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="6"/>
       <c r="C173" s="4"/>
       <c r="D173" s="1"/>
-    </row>
-    <row r="174" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E173" s="1" t="str">
+        <f>IF(D173="", "", SUM(D$3:D173))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="174" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
       <c r="C174" s="4"/>
       <c r="D174" s="1"/>
-    </row>
-    <row r="175" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E174" s="1" t="str">
+        <f>IF(D174="", "", SUM(D$3:D174))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="175" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="6"/>
       <c r="C175" s="4"/>
       <c r="D175" s="1"/>
-    </row>
-    <row r="176" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E175" s="1" t="str">
+        <f>IF(D175="", "", SUM(D$3:D175))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="176" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="6"/>
       <c r="C176" s="4"/>
       <c r="D176" s="1"/>
-    </row>
-    <row r="177" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E176" s="1" t="str">
+        <f>IF(D176="", "", SUM(D$3:D176))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="177" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="6"/>
       <c r="C177" s="4"/>
       <c r="D177" s="1"/>
-    </row>
-    <row r="178" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E177" s="1" t="str">
+        <f>IF(D177="", "", SUM(D$3:D177))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="178" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
       <c r="C178" s="4"/>
       <c r="D178" s="1"/>
-    </row>
-    <row r="179" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E178" s="1" t="str">
+        <f>IF(D178="", "", SUM(D$3:D178))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
       <c r="C179" s="4"/>
       <c r="D179" s="1"/>
-    </row>
-    <row r="180" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E179" s="1" t="str">
+        <f>IF(D179="", "", SUM(D$3:D179))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="6"/>
       <c r="C180" s="4"/>
       <c r="D180" s="1"/>
-    </row>
-    <row r="181" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E180" s="1" t="str">
+        <f>IF(D180="", "", SUM(D$3:D180))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="181" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="6"/>
       <c r="C181" s="4"/>
       <c r="D181" s="1"/>
-    </row>
-    <row r="182" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E181" s="1" t="str">
+        <f>IF(D181="", "", SUM(D$3:D181))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="182" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="6"/>
       <c r="C182" s="4"/>
       <c r="D182" s="1"/>
-    </row>
-    <row r="183" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E182" s="1" t="str">
+        <f>IF(D182="", "", SUM(D$3:D182))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
       <c r="C183" s="4"/>
       <c r="D183" s="1"/>
-    </row>
-    <row r="184" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E183" s="1" t="str">
+        <f>IF(D183="", "", SUM(D$3:D183))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="184" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="6"/>
       <c r="C184" s="4"/>
       <c r="D184" s="1"/>
-    </row>
-    <row r="185" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E184" s="1" t="str">
+        <f>IF(D184="", "", SUM(D$3:D184))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="6"/>
       <c r="C185" s="4"/>
       <c r="D185" s="1"/>
-    </row>
-    <row r="186" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E185" s="1" t="str">
+        <f>IF(D185="", "", SUM(D$3:D185))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="186" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
       <c r="C186" s="4"/>
       <c r="D186" s="1"/>
-    </row>
-    <row r="187" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E186" s="1" t="str">
+        <f>IF(D186="", "", SUM(D$3:D186))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
       <c r="C187" s="4"/>
       <c r="D187" s="1"/>
-    </row>
-    <row r="188" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E187" s="1" t="str">
+        <f>IF(D187="", "", SUM(D$3:D187))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
       <c r="C188" s="4"/>
       <c r="D188" s="1"/>
-    </row>
-    <row r="189" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E188" s="1" t="str">
+        <f>IF(D188="", "", SUM(D$3:D188))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="6"/>
       <c r="C189" s="4"/>
       <c r="D189" s="1"/>
-    </row>
-    <row r="190" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E189" s="1" t="str">
+        <f>IF(D189="", "", SUM(D$3:D189))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="6"/>
       <c r="C190" s="4"/>
       <c r="D190" s="1"/>
-    </row>
-    <row r="191" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E190" s="1" t="str">
+        <f>IF(D190="", "", SUM(D$3:D190))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="6"/>
       <c r="C191" s="4"/>
       <c r="D191" s="1"/>
-    </row>
-    <row r="192" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E191" s="1" t="str">
+        <f>IF(D191="", "", SUM(D$3:D191))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="192" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="6"/>
       <c r="C192" s="4"/>
       <c r="D192" s="1"/>
-    </row>
-    <row r="193" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E192" s="1" t="str">
+        <f>IF(D192="", "", SUM(D$3:D192))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="6"/>
       <c r="C193" s="4"/>
       <c r="D193" s="1"/>
-    </row>
-    <row r="194" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E193" s="1" t="str">
+        <f>IF(D193="", "", SUM(D$3:D193))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="194" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="6"/>
       <c r="C194" s="4"/>
       <c r="D194" s="1"/>
-    </row>
-    <row r="195" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E194" s="1" t="str">
+        <f>IF(D194="", "", SUM(D$3:D194))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="195" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
       <c r="C195" s="4"/>
       <c r="D195" s="1"/>
-    </row>
-    <row r="196" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E195" s="1" t="str">
+        <f>IF(D195="", "", SUM(D$3:D195))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="196" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="6"/>
       <c r="C196" s="4"/>
       <c r="D196" s="1"/>
-    </row>
-    <row r="197" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E196" s="1" t="str">
+        <f>IF(D196="", "", SUM(D$3:D196))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="197" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="6"/>
       <c r="C197" s="4"/>
       <c r="D197" s="1"/>
-    </row>
-    <row r="198" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E197" s="1" t="str">
+        <f>IF(D197="", "", SUM(D$3:D197))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="198" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="6"/>
       <c r="C198" s="4"/>
       <c r="D198" s="1"/>
-    </row>
-    <row r="199" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E198" s="1" t="str">
+        <f>IF(D198="", "", SUM(D$3:D198))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="199" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="6"/>
       <c r="C199" s="4"/>
       <c r="D199" s="1"/>
-    </row>
-    <row r="200" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E199" s="1" t="str">
+        <f>IF(D199="", "", SUM(D$3:D199))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="200" spans="2:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="7"/>
       <c r="C200" s="4"/>
       <c r="D200" s="1"/>
+      <c r="E200" s="1" t="str">
+        <f>IF(D200="", "", SUM(D$3:D200))</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixing and tweaking fight behavior
Created a fight script to ease the process + fixed behavior to take some
neglected scenarii (if target goes behind a wall after opening fire for
example); now works as intended no matter what
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Enhanced shooting behavior</t>
+  </si>
+  <si>
+    <t>Tweaking and fixing fight behaviors</t>
   </si>
 </sst>
 </file>
@@ -159,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -186,6 +189,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -495,7 +501,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +544,7 @@
       </c>
       <c r="G3" s="1">
         <f>SUM(D3:D200)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -568,12 +574,16 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="str">
+      <c r="B6" s="10"/>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <f>IF(D6="", "", SUM(D$3:D6))</f>
-        <v/>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2324,7 +2334,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B3:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed architecture to use classes inheritence + added AI behavior state machine
Now scripts are well organized;
Now AI behavior can be set either on agressive, defensive or coward
(respectively: attack on sight, attack if attacked and flee if attacked)
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -43,6 +43,9 @@
   <si>
     <t>Tweaking and fixing fight behaviors</t>
   </si>
+  <si>
+    <t>Changed architecture to use classes inheritence + added behavior state machine (coward, agressive and defensive)</t>
+  </si>
 </sst>
 </file>
 
@@ -65,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,6 +84,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -162,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -192,6 +201,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -501,13 +513,13 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="100.7109375" customWidth="1"/>
+    <col min="3" max="3" width="108.85546875" customWidth="1"/>
     <col min="4" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -544,7 +556,7 @@
       </c>
       <c r="G3" s="1">
         <f>SUM(D3:D200)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -587,12 +599,18 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="str">
+      <c r="B7" s="11">
+        <v>42301</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
         <f>IF(D7="", "", SUM(D$3:D7))</f>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Integrated building + made roof disappear if player inside
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Changed architecture to use classes inheritence + added behavior state machine (coward, agressive and defensive)</t>
+  </si>
+  <si>
+    <t>Basic building mod + integration</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,6 +207,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -513,7 +519,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +562,7 @@
       </c>
       <c r="G3" s="1">
         <f>SUM(D3:D200)</f>
-        <v>5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -599,7 +605,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+      <c r="B7" s="12">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -614,12 +620,16 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="str">
+      <c r="B8" s="11"/>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="1">
         <f>IF(D8="", "", SUM(D$3:D8))</f>
-        <v/>
+        <v>5.5</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2351,8 +2361,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added custom shader to render characters behind walls
Now, if a character goes behind an opaque obstacle, he will be rendered
in unlit colors through the obstacle.
It was shader class today and I was ahead of time so..
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Basic building mod + integration</t>
+  </si>
+  <si>
+    <t>Made custom shader and logic to display characters behind walls by transparency</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,10 +209,13 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -519,7 +525,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +568,7 @@
       </c>
       <c r="G3" s="1">
         <f>SUM(D3:D200)</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -605,7 +611,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -620,7 +626,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -633,12 +639,16 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="str">
+      <c r="B9" s="13"/>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
         <f>IF(D9="", "", SUM(D$3:D9))</f>
-        <v/>
+        <v>8.5</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2363,7 +2373,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added HUD with selection and health-bar update
Now character can be selected and deselected and HUD is updated
accordingly
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Made custom shader and logic to display characters behind walls by transparency</t>
+  </si>
+  <si>
+    <t>Trying to figure out how UI elements work in Unity + designed and integrated HUD (functionnal)</t>
   </si>
 </sst>
 </file>
@@ -177,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -198,6 +201,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -524,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +559,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8">
+      <c r="B3" s="9">
         <v>42300</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -568,11 +574,11 @@
       </c>
       <c r="G3" s="1">
         <f>SUM(D3:D200)</f>
-        <v>8.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -585,7 +591,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -598,7 +604,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
@@ -611,7 +617,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+      <c r="B7" s="12">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -626,7 +632,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -639,7 +645,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
@@ -652,12 +658,18 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="str">
+      <c r="B10" s="8">
+        <v>42302</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E10" s="1">
         <f>IF(D10="", "", SUM(D$3:D10))</f>
-        <v/>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed some more HUD issues + designed basic map
Selection buttons for characters 2 3 4 were misplaced and had to be
tweaked.
Now HUD works fine and able to control characters as intended (though
they currently don't position themselves right when going somewhere
together)
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Added main title menu scene</t>
+  </si>
+  <si>
+    <t>Fixed some more HUD issues and designed basic map</t>
   </si>
 </sst>
 </file>
@@ -533,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +580,7 @@
       </c>
       <c r="G3" s="1">
         <f>SUM(D3:D200)</f>
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -702,12 +705,16 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="str">
+      <c r="B13" s="9"/>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
         <f>IF(D13="", "", SUM(D$3:D13))</f>
-        <v/>
+        <v>15.5</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2397,7 +2404,7 @@
   <mergeCells count="3">
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Reorganized hierarchy and some code + added wandering behavior + added civilians
Now able to set npcs to three wandering behaviours: no wandering, area
wandering and wander anywhere
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Finished minimap (added buildings and walls blips + rotation)</t>
+  </si>
+  <si>
+    <t>Reorganized code and objects hierarchy</t>
+  </si>
+  <si>
+    <t>Added wandering behaviour + created civilians</t>
   </si>
 </sst>
 </file>
@@ -233,6 +239,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -240,12 +252,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -581,7 +587,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +618,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="B3" s="11">
         <v>42300</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -631,11 +637,11 @@
       </c>
       <c r="G3" s="8">
         <f>SUM(D3:D200)</f>
-        <v>21.5</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -649,7 +655,7 @@
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -663,7 +669,7 @@
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
@@ -677,7 +683,7 @@
       <c r="F6" s="17"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -696,7 +702,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -724,7 +730,7 @@
       <c r="F9" s="20"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+      <c r="B10" s="11">
         <v>42302</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -743,7 +749,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
@@ -757,7 +763,7 @@
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -771,7 +777,7 @@
       <c r="F12" s="16"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
@@ -785,7 +791,7 @@
       <c r="F13" s="16"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
@@ -799,7 +805,7 @@
       <c r="F14" s="17"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
+      <c r="B15" s="9">
         <v>42303</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -815,7 +821,7 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
@@ -829,22 +835,30 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="str">
+      <c r="B17" s="10"/>
+      <c r="C17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
         <f>IF(D17="", "", SUM(D$3:D17))</f>
-        <v/>
+        <v>23.5</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="str">
+      <c r="B18" s="10"/>
+      <c r="C18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
         <f>IF(D18="", "", SUM(D$3:D18))</f>
-        <v/>
+        <v>24.5</v>
       </c>
       <c r="F18" s="6"/>
     </row>
@@ -2670,13 +2684,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B15:B16"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="F10:F14"/>
+    <mergeCell ref="B15:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added civilians and enemies procedural generation + fixed minor bugs
- Fixed targetting behaviour (didn't always lose target when it died)
- Fixed blips (to be pointed only when enemy is a target)
- Slight changes in variables names and organization
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Added wandering behaviour + created civilians</t>
+  </si>
+  <si>
+    <t>Working on civilians and bad guys procedular generation (but got unexplained issues so far)</t>
+  </si>
+  <si>
+    <t>Fixed civilians and bad guys generation</t>
   </si>
 </sst>
 </file>
@@ -213,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -239,10 +245,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -252,9 +264,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -586,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +627,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11">
+      <c r="B3" s="13">
         <v>42300</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -631,17 +640,17 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>0.5</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="16">
         <f>SUM(D3:D6)</f>
         <v>3</v>
       </c>
       <c r="G3" s="8">
         <f>SUM(D3:D200)</f>
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -652,10 +661,10 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>1.5</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -666,10 +675,10 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>2</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
@@ -680,10 +689,10 @@
         <f>IF(D6="", "", SUM(D$3:D6))</f>
         <v>3</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="B7" s="10">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -696,13 +705,13 @@
         <f>IF(D7="", "", SUM(D$3:D7))</f>
         <v>5</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="19">
         <f>SUM(D7:D9)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -713,10 +722,10 @@
         <f>IF(D8="", "", SUM(D$3:D8))</f>
         <v>5.5</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
@@ -727,10 +736,10 @@
         <f>IF(D9="", "", SUM(D$3:D9))</f>
         <v>8.5</v>
       </c>
-      <c r="F9" s="20"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
+      <c r="B10" s="13">
         <v>42302</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -743,13 +752,13 @@
         <f>IF(D10="", "", SUM(D$3:D10))</f>
         <v>12</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="16">
         <f>SUM(D10:D14)</f>
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
@@ -760,10 +769,10 @@
         <f>IF(D11="", "", SUM(D$3:D11))</f>
         <v>14</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -774,10 +783,10 @@
         <f>IF(D12="", "", SUM(D$3:D12))</f>
         <v>14.5</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
@@ -788,10 +797,10 @@
         <f>IF(D13="", "", SUM(D$3:D13))</f>
         <v>15.5</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
@@ -802,10 +811,10 @@
         <f>IF(D14="", "", SUM(D$3:D14))</f>
         <v>17.5</v>
       </c>
-      <c r="F14" s="17"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="9">
+      <c r="B15" s="10">
         <v>42303</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -818,10 +827,13 @@
         <f>IF(D15="", "", SUM(D$3:D15))</f>
         <v>19.5</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="19">
+        <f>SUM(D15:D19)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
@@ -832,10 +844,10 @@
         <f>IF(D16="", "", SUM(D$3:D16))</f>
         <v>21.5</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
@@ -846,10 +858,10 @@
         <f>IF(D17="", "", SUM(D$3:D17))</f>
         <v>23.5</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="20"/>
     </row>
     <row r="18" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -860,25 +872,35 @@
         <f>IF(D18="", "", SUM(D$3:D18))</f>
         <v>24.5</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="str">
+      <c r="B19" s="12"/>
+      <c r="C19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
         <f>IF(D19="", "", SUM(D$3:D19))</f>
-        <v/>
-      </c>
-      <c r="F19" s="6"/>
+        <v>25.5</v>
+      </c>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="str">
+      <c r="B20" s="9">
+        <v>42304</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
         <f>IF(D20="", "", SUM(D$3:D20))</f>
-        <v/>
+        <v>26.5</v>
       </c>
       <c r="F20" s="6"/>
     </row>
@@ -2683,14 +2705,15 @@
       <c r="F200" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B15:B19"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="F10:F14"/>
-    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="F15:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added multiple characters control + fixed bugs and refactored some code
- Now selection works better (able to select characters by clicking them
in the world) + when assigning a destination, characters will organize
to place themselves in a line
- Fixed various bugs and malfunctions (characters shooting through walls
or at infinite distance, characters were able to kill each other (now if
they shoot each other by mistake they will "argue" but doing no damage -
need to add ability to find nearby allies's target to help them), ...)
- Reorganised some code (added OnDeath() callback + various other
changes and fixes)
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Started adding weapons (only hand gun for now)</t>
+  </si>
+  <si>
+    <t>Added multiple characters control</t>
+  </si>
+  <si>
+    <t>Fixed bugs and reorganized some code</t>
   </si>
 </sst>
 </file>
@@ -254,24 +260,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -288,6 +276,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -601,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +639,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="B3" s="15">
         <v>42300</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -646,17 +652,17 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>0.5</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="9">
         <f>SUM(D3:D6)</f>
         <v>3</v>
       </c>
       <c r="G3" s="8">
         <f>SUM(D3:D200)</f>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -667,10 +673,10 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>1.5</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -681,10 +687,10 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>2</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
@@ -695,10 +701,10 @@
         <f>IF(D6="", "", SUM(D$3:D6))</f>
         <v>3</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+      <c r="B7" s="18">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -711,13 +717,13 @@
         <f>IF(D7="", "", SUM(D$3:D7))</f>
         <v>5</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="12">
         <f>SUM(D7:D9)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -728,10 +734,10 @@
         <f>IF(D8="", "", SUM(D$3:D8))</f>
         <v>5.5</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
@@ -742,10 +748,10 @@
         <f>IF(D9="", "", SUM(D$3:D9))</f>
         <v>8.5</v>
       </c>
-      <c r="F9" s="20"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+      <c r="B10" s="15">
         <v>42302</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -758,13 +764,13 @@
         <f>IF(D10="", "", SUM(D$3:D10))</f>
         <v>12</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="9">
         <f>SUM(D10:D14)</f>
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
@@ -775,10 +781,10 @@
         <f>IF(D11="", "", SUM(D$3:D11))</f>
         <v>14</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -789,10 +795,10 @@
         <f>IF(D12="", "", SUM(D$3:D12))</f>
         <v>14.5</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
@@ -803,10 +809,10 @@
         <f>IF(D13="", "", SUM(D$3:D13))</f>
         <v>15.5</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
@@ -817,10 +823,10 @@
         <f>IF(D14="", "", SUM(D$3:D14))</f>
         <v>17.5</v>
       </c>
-      <c r="F14" s="17"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11">
+      <c r="B15" s="18">
         <v>42303</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -833,13 +839,13 @@
         <f>IF(D15="", "", SUM(D$3:D15))</f>
         <v>19.5</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="12">
         <f>SUM(D15:D19)</f>
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
@@ -850,10 +856,10 @@
         <f>IF(D16="", "", SUM(D$3:D16))</f>
         <v>21.5</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
@@ -864,10 +870,10 @@
         <f>IF(D17="", "", SUM(D$3:D17))</f>
         <v>23.5</v>
       </c>
-      <c r="F17" s="19"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -878,10 +884,10 @@
         <f>IF(D18="", "", SUM(D$3:D18))</f>
         <v>24.5</v>
       </c>
-      <c r="F18" s="19"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
@@ -892,10 +898,10 @@
         <f>IF(D19="", "", SUM(D$3:D19))</f>
         <v>25.5</v>
       </c>
-      <c r="F19" s="20"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="9">
+      <c r="B20" s="15">
         <v>42304</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -908,13 +914,13 @@
         <f>IF(D20="", "", SUM(D$3:D20))</f>
         <v>26.5</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="9">
         <f>SUM(D20:D23)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="4" t="s">
         <v>24</v>
       </c>
@@ -925,10 +931,10 @@
         <f>IF(D21="", "", SUM(D$3:D21))</f>
         <v>27.5</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="4" t="s">
         <v>25</v>
       </c>
@@ -939,10 +945,10 @@
         <f>IF(D22="", "", SUM(D$3:D22))</f>
         <v>28</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="4" t="s">
         <v>26</v>
       </c>
@@ -953,25 +959,35 @@
         <f>IF(D23="", "", SUM(D$3:D23))</f>
         <v>29</v>
       </c>
-      <c r="F23" s="17"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1" t="str">
+      <c r="B24" s="18">
+        <v>42305</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
         <f>IF(D24="", "", SUM(D$3:D24))</f>
-        <v/>
+        <v>30</v>
       </c>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1" t="str">
+      <c r="B25" s="19"/>
+      <c r="C25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
         <f>IF(D25="", "", SUM(D$3:D25))</f>
-        <v/>
+        <v>33</v>
       </c>
       <c r="F25" s="6"/>
     </row>
@@ -2726,7 +2742,8 @@
       <c r="F200" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="F10:F14"/>

</xml_diff>

<commit_message>
Added inventory selection sprite to know which weapon is currently selected
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Fixed SendDirection() and refactored a bit</t>
+  </si>
+  <si>
+    <t>Added inventory selection sprite to know which weapon is selected</t>
   </si>
 </sst>
 </file>
@@ -269,6 +272,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -294,12 +303,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -617,7 +620,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +651,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18">
+      <c r="B3" s="9">
         <v>42300</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -661,17 +664,17 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>0.5</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="17">
         <f>SUM(D3:D6)</f>
         <v>3</v>
       </c>
       <c r="G3" s="8">
         <f>SUM(D3:D200)</f>
-        <v>37.5</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -682,10 +685,10 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>1.5</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -696,7 +699,7 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>2</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
@@ -710,10 +713,10 @@
         <f>IF(D6="", "", SUM(D$3:D6))</f>
         <v>3</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="B7" s="11">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -726,13 +729,13 @@
         <f>IF(D7="", "", SUM(D$3:D7))</f>
         <v>5</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="14">
         <f>SUM(D7:D9)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -743,10 +746,10 @@
         <f>IF(D8="", "", SUM(D$3:D8))</f>
         <v>5.5</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
@@ -757,10 +760,10 @@
         <f>IF(D9="", "", SUM(D$3:D9))</f>
         <v>8.5</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="18">
+      <c r="B10" s="9">
         <v>42302</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -773,13 +776,13 @@
         <f>IF(D10="", "", SUM(D$3:D10))</f>
         <v>12</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="17">
         <f>SUM(D10:D14)</f>
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
@@ -790,10 +793,10 @@
         <f>IF(D11="", "", SUM(D$3:D11))</f>
         <v>14</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -804,10 +807,10 @@
         <f>IF(D12="", "", SUM(D$3:D12))</f>
         <v>14.5</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
@@ -818,7 +821,7 @@
         <f>IF(D13="", "", SUM(D$3:D13))</f>
         <v>15.5</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20"/>
@@ -832,10 +835,10 @@
         <f>IF(D14="", "", SUM(D$3:D14))</f>
         <v>17.5</v>
       </c>
-      <c r="F14" s="17"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="9">
+      <c r="B15" s="11">
         <v>42303</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -848,13 +851,13 @@
         <f>IF(D15="", "", SUM(D$3:D15))</f>
         <v>19.5</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="14">
         <f>SUM(D15:D19)</f>
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
@@ -865,10 +868,10 @@
         <f>IF(D16="", "", SUM(D$3:D16))</f>
         <v>21.5</v>
       </c>
-      <c r="F16" s="13"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
@@ -879,10 +882,10 @@
         <f>IF(D17="", "", SUM(D$3:D17))</f>
         <v>23.5</v>
       </c>
-      <c r="F17" s="13"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -893,10 +896,10 @@
         <f>IF(D18="", "", SUM(D$3:D18))</f>
         <v>24.5</v>
       </c>
-      <c r="F18" s="13"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
@@ -907,10 +910,10 @@
         <f>IF(D19="", "", SUM(D$3:D19))</f>
         <v>25.5</v>
       </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="18">
+      <c r="B20" s="9">
         <v>42304</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -923,13 +926,13 @@
         <f>IF(D20="", "", SUM(D$3:D20))</f>
         <v>26.5</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="17">
         <f>SUM(D20:D23)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="4" t="s">
         <v>24</v>
       </c>
@@ -940,10 +943,10 @@
         <f>IF(D21="", "", SUM(D$3:D21))</f>
         <v>27.5</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="4" t="s">
         <v>25</v>
       </c>
@@ -954,7 +957,7 @@
         <f>IF(D22="", "", SUM(D$3:D22))</f>
         <v>28</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
@@ -968,10 +971,10 @@
         <f>IF(D23="", "", SUM(D$3:D23))</f>
         <v>29</v>
       </c>
-      <c r="F23" s="17"/>
+      <c r="F23" s="19"/>
     </row>
     <row r="24" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="9">
+      <c r="B24" s="11">
         <v>42305</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -984,13 +987,13 @@
         <f>IF(D24="", "", SUM(D$3:D24))</f>
         <v>30</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="14">
         <f>SUM(D24:D26)</f>
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="4" t="s">
         <v>28</v>
       </c>
@@ -1001,10 +1004,10 @@
         <f>IF(D25="", "", SUM(D$3:D25))</f>
         <v>33</v>
       </c>
-      <c r="F25" s="13"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="4" t="s">
         <v>29</v>
       </c>
@@ -1015,10 +1018,10 @@
         <f>IF(D26="", "", SUM(D$3:D26))</f>
         <v>35</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="18">
+      <c r="B27" s="9">
         <v>42306</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1034,7 +1037,7 @@
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
@@ -1048,12 +1051,16 @@
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1" t="str">
+      <c r="B29" s="10"/>
+      <c r="C29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
         <f>IF(D29="", "", SUM(D$3:D29))</f>
-        <v/>
+        <v>38.5</v>
       </c>
       <c r="F29" s="6"/>
     </row>
@@ -2769,7 +2776,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B27:B28"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="F24:F26"/>
     <mergeCell ref="F3:F6"/>
@@ -2782,6 +2788,7 @@
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B27:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed characters selection + fixed characters AI
- Now selecting a character will enable the right selection gizmo
- Fixed characters AI behaviour where they attacked target before
checking if target was dead
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Added inventory selection sprite to know which weapon is selected</t>
+  </si>
+  <si>
+    <t>Fixed selection order (buttons that did not select right player) + fixed characters AI behaviour</t>
   </si>
 </sst>
 </file>
@@ -272,12 +275,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -303,6 +300,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -619,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +654,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="B3" s="18">
         <v>42300</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -664,17 +667,17 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>0.5</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="15">
         <f>SUM(D3:D6)</f>
         <v>3</v>
       </c>
       <c r="G3" s="8">
         <f>SUM(D3:D200)</f>
-        <v>38.5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -685,10 +688,10 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>1.5</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -699,7 +702,7 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>2</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
@@ -713,10 +716,10 @@
         <f>IF(D6="", "", SUM(D$3:D6))</f>
         <v>3</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -729,13 +732,13 @@
         <f>IF(D7="", "", SUM(D$3:D7))</f>
         <v>5</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="12">
         <f>SUM(D7:D9)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -746,10 +749,10 @@
         <f>IF(D8="", "", SUM(D$3:D8))</f>
         <v>5.5</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
@@ -760,10 +763,10 @@
         <f>IF(D9="", "", SUM(D$3:D9))</f>
         <v>8.5</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+      <c r="B10" s="18">
         <v>42302</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -776,13 +779,13 @@
         <f>IF(D10="", "", SUM(D$3:D10))</f>
         <v>12</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="15">
         <f>SUM(D10:D14)</f>
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
@@ -793,10 +796,10 @@
         <f>IF(D11="", "", SUM(D$3:D11))</f>
         <v>14</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -807,10 +810,10 @@
         <f>IF(D12="", "", SUM(D$3:D12))</f>
         <v>14.5</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
@@ -821,7 +824,7 @@
         <f>IF(D13="", "", SUM(D$3:D13))</f>
         <v>15.5</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20"/>
@@ -835,10 +838,10 @@
         <f>IF(D14="", "", SUM(D$3:D14))</f>
         <v>17.5</v>
       </c>
-      <c r="F14" s="19"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11">
+      <c r="B15" s="9">
         <v>42303</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -851,13 +854,13 @@
         <f>IF(D15="", "", SUM(D$3:D15))</f>
         <v>19.5</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="12">
         <f>SUM(D15:D19)</f>
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
@@ -868,10 +871,10 @@
         <f>IF(D16="", "", SUM(D$3:D16))</f>
         <v>21.5</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
@@ -882,10 +885,10 @@
         <f>IF(D17="", "", SUM(D$3:D17))</f>
         <v>23.5</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -896,10 +899,10 @@
         <f>IF(D18="", "", SUM(D$3:D18))</f>
         <v>24.5</v>
       </c>
-      <c r="F18" s="15"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
@@ -910,10 +913,10 @@
         <f>IF(D19="", "", SUM(D$3:D19))</f>
         <v>25.5</v>
       </c>
-      <c r="F19" s="16"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="9">
+      <c r="B20" s="18">
         <v>42304</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -926,13 +929,13 @@
         <f>IF(D20="", "", SUM(D$3:D20))</f>
         <v>26.5</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="15">
         <f>SUM(D20:D23)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="4" t="s">
         <v>24</v>
       </c>
@@ -943,10 +946,10 @@
         <f>IF(D21="", "", SUM(D$3:D21))</f>
         <v>27.5</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="4" t="s">
         <v>25</v>
       </c>
@@ -957,7 +960,7 @@
         <f>IF(D22="", "", SUM(D$3:D22))</f>
         <v>28</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
@@ -971,10 +974,10 @@
         <f>IF(D23="", "", SUM(D$3:D23))</f>
         <v>29</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="11">
+      <c r="B24" s="9">
         <v>42305</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -987,13 +990,13 @@
         <f>IF(D24="", "", SUM(D$3:D24))</f>
         <v>30</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="12">
         <f>SUM(D24:D26)</f>
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="4" t="s">
         <v>28</v>
       </c>
@@ -1004,10 +1007,10 @@
         <f>IF(D25="", "", SUM(D$3:D25))</f>
         <v>33</v>
       </c>
-      <c r="F25" s="15"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="4" t="s">
         <v>29</v>
       </c>
@@ -1018,10 +1021,10 @@
         <f>IF(D26="", "", SUM(D$3:D26))</f>
         <v>35</v>
       </c>
-      <c r="F26" s="16"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="9">
+      <c r="B27" s="18">
         <v>42306</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1037,7 +1040,7 @@
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
@@ -1051,7 +1054,7 @@
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="4" t="s">
         <v>32</v>
       </c>
@@ -1065,12 +1068,16 @@
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1" t="str">
+      <c r="B30" s="19"/>
+      <c r="C30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="1">
         <f>IF(D30="", "", SUM(D$3:D30))</f>
-        <v/>
+        <v>39</v>
       </c>
       <c r="F30" s="6"/>
     </row>
@@ -2776,6 +2783,7 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B27:B30"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="F24:F26"/>
     <mergeCell ref="F3:F6"/>
@@ -2788,7 +2796,6 @@
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B27:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added persuador and persuaded behaviour
Now able to select and use persuador to turn ennemies into allies with
certain persuasion difficulty and persuaded npcs will follow nearest
player and flee (if no weapon equipped) or help player if a fight get
started
+ fixed behaviour -> now if a normally agressive character doesn't have
an active weapon, it will flee if attacked, as intended
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Fixed selection order (buttons that did not select right player) + fixed characters AI behaviour</t>
+  </si>
+  <si>
+    <t>Added persuador and persuaded behavior</t>
   </si>
 </sst>
 </file>
@@ -275,6 +278,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -300,12 +309,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -623,7 +626,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B30"/>
+      <selection activeCell="B27" sqref="B27:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +657,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18">
+      <c r="B3" s="9">
         <v>42300</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -667,17 +670,17 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>0.5</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="17">
         <f>SUM(D3:D6)</f>
         <v>3</v>
       </c>
       <c r="G3" s="8">
         <f>SUM(D3:D200)</f>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -688,10 +691,10 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>1.5</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -702,7 +705,7 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>2</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
@@ -716,10 +719,10 @@
         <f>IF(D6="", "", SUM(D$3:D6))</f>
         <v>3</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="B7" s="11">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -732,13 +735,13 @@
         <f>IF(D7="", "", SUM(D$3:D7))</f>
         <v>5</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="14">
         <f>SUM(D7:D9)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -749,10 +752,10 @@
         <f>IF(D8="", "", SUM(D$3:D8))</f>
         <v>5.5</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
@@ -763,10 +766,10 @@
         <f>IF(D9="", "", SUM(D$3:D9))</f>
         <v>8.5</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="18">
+      <c r="B10" s="9">
         <v>42302</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -779,13 +782,13 @@
         <f>IF(D10="", "", SUM(D$3:D10))</f>
         <v>12</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="17">
         <f>SUM(D10:D14)</f>
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
@@ -796,10 +799,10 @@
         <f>IF(D11="", "", SUM(D$3:D11))</f>
         <v>14</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -810,10 +813,10 @@
         <f>IF(D12="", "", SUM(D$3:D12))</f>
         <v>14.5</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
@@ -824,7 +827,7 @@
         <f>IF(D13="", "", SUM(D$3:D13))</f>
         <v>15.5</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20"/>
@@ -838,10 +841,10 @@
         <f>IF(D14="", "", SUM(D$3:D14))</f>
         <v>17.5</v>
       </c>
-      <c r="F14" s="17"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="9">
+      <c r="B15" s="11">
         <v>42303</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -854,13 +857,13 @@
         <f>IF(D15="", "", SUM(D$3:D15))</f>
         <v>19.5</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="14">
         <f>SUM(D15:D19)</f>
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
@@ -871,10 +874,10 @@
         <f>IF(D16="", "", SUM(D$3:D16))</f>
         <v>21.5</v>
       </c>
-      <c r="F16" s="13"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
@@ -885,10 +888,10 @@
         <f>IF(D17="", "", SUM(D$3:D17))</f>
         <v>23.5</v>
       </c>
-      <c r="F17" s="13"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -899,10 +902,10 @@
         <f>IF(D18="", "", SUM(D$3:D18))</f>
         <v>24.5</v>
       </c>
-      <c r="F18" s="13"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
@@ -913,10 +916,10 @@
         <f>IF(D19="", "", SUM(D$3:D19))</f>
         <v>25.5</v>
       </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="18">
+      <c r="B20" s="9">
         <v>42304</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -929,13 +932,13 @@
         <f>IF(D20="", "", SUM(D$3:D20))</f>
         <v>26.5</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="17">
         <f>SUM(D20:D23)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="4" t="s">
         <v>24</v>
       </c>
@@ -946,10 +949,10 @@
         <f>IF(D21="", "", SUM(D$3:D21))</f>
         <v>27.5</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="4" t="s">
         <v>25</v>
       </c>
@@ -960,7 +963,7 @@
         <f>IF(D22="", "", SUM(D$3:D22))</f>
         <v>28</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
@@ -974,10 +977,10 @@
         <f>IF(D23="", "", SUM(D$3:D23))</f>
         <v>29</v>
       </c>
-      <c r="F23" s="17"/>
+      <c r="F23" s="19"/>
     </row>
     <row r="24" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="9">
+      <c r="B24" s="11">
         <v>42305</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -990,13 +993,13 @@
         <f>IF(D24="", "", SUM(D$3:D24))</f>
         <v>30</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="14">
         <f>SUM(D24:D26)</f>
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="4" t="s">
         <v>28</v>
       </c>
@@ -1007,10 +1010,10 @@
         <f>IF(D25="", "", SUM(D$3:D25))</f>
         <v>33</v>
       </c>
-      <c r="F25" s="13"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="4" t="s">
         <v>29</v>
       </c>
@@ -1021,10 +1024,10 @@
         <f>IF(D26="", "", SUM(D$3:D26))</f>
         <v>35</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="18">
+      <c r="B27" s="9">
         <v>42306</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1040,7 +1043,7 @@
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
@@ -1054,7 +1057,7 @@
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="4" t="s">
         <v>32</v>
       </c>
@@ -1068,7 +1071,7 @@
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1082,12 +1085,16 @@
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1" t="str">
+      <c r="B31" s="10"/>
+      <c r="C31" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1">
         <f>IF(D31="", "", SUM(D$3:D31))</f>
-        <v/>
+        <v>41</v>
       </c>
       <c r="F31" s="6"/>
     </row>
@@ -2783,7 +2790,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B27:B30"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="F24:F26"/>
     <mergeCell ref="F3:F6"/>
@@ -2796,6 +2802,7 @@
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B27:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added choose mission menu + added persuade mission + added camera shake when someone hit
</commit_message>
<xml_diff>
--- a/Syndicate_Recreate/Time tracking.xlsx
+++ b/Syndicate_Recreate/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Added persuador and persuaded behavior</t>
+  </si>
+  <si>
+    <t>Added persuasion mission + mission selection</t>
+  </si>
+  <si>
+    <t>Added camera shake</t>
   </si>
 </sst>
 </file>
@@ -278,12 +284,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -309,6 +309,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -626,7 +632,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B31"/>
+      <selection activeCell="B27" sqref="B27:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +663,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="B3" s="18">
         <v>42300</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -670,17 +676,17 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>0.5</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="15">
         <f>SUM(D3:D6)</f>
         <v>3</v>
       </c>
       <c r="G3" s="8">
         <f>SUM(D3:D200)</f>
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -691,10 +697,10 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>1.5</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -705,7 +711,7 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>2</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
@@ -719,10 +725,10 @@
         <f>IF(D6="", "", SUM(D$3:D6))</f>
         <v>3</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>42301</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -735,13 +741,13 @@
         <f>IF(D7="", "", SUM(D$3:D7))</f>
         <v>5</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="12">
         <f>SUM(D7:D9)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -752,10 +758,10 @@
         <f>IF(D8="", "", SUM(D$3:D8))</f>
         <v>5.5</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
@@ -766,10 +772,10 @@
         <f>IF(D9="", "", SUM(D$3:D9))</f>
         <v>8.5</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+      <c r="B10" s="18">
         <v>42302</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -782,13 +788,13 @@
         <f>IF(D10="", "", SUM(D$3:D10))</f>
         <v>12</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="15">
         <f>SUM(D10:D14)</f>
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
@@ -799,10 +805,10 @@
         <f>IF(D11="", "", SUM(D$3:D11))</f>
         <v>14</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -813,10 +819,10 @@
         <f>IF(D12="", "", SUM(D$3:D12))</f>
         <v>14.5</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
@@ -827,7 +833,7 @@
         <f>IF(D13="", "", SUM(D$3:D13))</f>
         <v>15.5</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20"/>
@@ -841,10 +847,10 @@
         <f>IF(D14="", "", SUM(D$3:D14))</f>
         <v>17.5</v>
       </c>
-      <c r="F14" s="19"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11">
+      <c r="B15" s="9">
         <v>42303</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -857,13 +863,13 @@
         <f>IF(D15="", "", SUM(D$3:D15))</f>
         <v>19.5</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="12">
         <f>SUM(D15:D19)</f>
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
@@ -874,10 +880,10 @@
         <f>IF(D16="", "", SUM(D$3:D16))</f>
         <v>21.5</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
@@ -888,10 +894,10 @@
         <f>IF(D17="", "", SUM(D$3:D17))</f>
         <v>23.5</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -902,10 +908,10 @@
         <f>IF(D18="", "", SUM(D$3:D18))</f>
         <v>24.5</v>
       </c>
-      <c r="F18" s="15"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
@@ -916,10 +922,10 @@
         <f>IF(D19="", "", SUM(D$3:D19))</f>
         <v>25.5</v>
       </c>
-      <c r="F19" s="16"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="9">
+      <c r="B20" s="18">
         <v>42304</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -932,13 +938,13 @@
         <f>IF(D20="", "", SUM(D$3:D20))</f>
         <v>26.5</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="15">
         <f>SUM(D20:D23)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="4" t="s">
         <v>24</v>
       </c>
@@ -949,10 +955,10 @@
         <f>IF(D21="", "", SUM(D$3:D21))</f>
         <v>27.5</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="4" t="s">
         <v>25</v>
       </c>
@@ -963,7 +969,7 @@
         <f>IF(D22="", "", SUM(D$3:D22))</f>
         <v>28</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
@@ -977,10 +983,10 @@
         <f>IF(D23="", "", SUM(D$3:D23))</f>
         <v>29</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="11">
+      <c r="B24" s="9">
         <v>42305</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -993,13 +999,13 @@
         <f>IF(D24="", "", SUM(D$3:D24))</f>
         <v>30</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="12">
         <f>SUM(D24:D26)</f>
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="4" t="s">
         <v>28</v>
       </c>
@@ -1010,10 +1016,10 @@
         <f>IF(D25="", "", SUM(D$3:D25))</f>
         <v>33</v>
       </c>
-      <c r="F25" s="15"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="4" t="s">
         <v>29</v>
       </c>
@@ -1024,10 +1030,10 @@
         <f>IF(D26="", "", SUM(D$3:D26))</f>
         <v>35</v>
       </c>
-      <c r="F26" s="16"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="9">
+      <c r="B27" s="18">
         <v>42306</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1043,7 +1049,7 @@
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
@@ -1057,7 +1063,7 @@
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="4" t="s">
         <v>32</v>
       </c>
@@ -1071,7 +1077,7 @@
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1085,7 +1091,7 @@
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1099,22 +1105,30 @@
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1" t="str">
+      <c r="B32" s="19"/>
+      <c r="C32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="1">
         <f>IF(D32="", "", SUM(D$3:D32))</f>
-        <v/>
+        <v>41.5</v>
       </c>
       <c r="F32" s="6"/>
     </row>
     <row r="33" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1" t="str">
+      <c r="B33" s="19"/>
+      <c r="C33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="1">
         <f>IF(D33="", "", SUM(D$3:D33))</f>
-        <v/>
+        <v>42</v>
       </c>
       <c r="F33" s="6"/>
     </row>
@@ -2790,6 +2804,7 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B27:B33"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="F24:F26"/>
     <mergeCell ref="F3:F6"/>
@@ -2802,7 +2817,6 @@
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B27:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>